<commit_message>
Added MGL checklist sources and corrected some spelling errors
</commit_message>
<xml_diff>
--- a/CHECKLIST.xlsx
+++ b/CHECKLIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weber/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56AC95D-9FE1-1D4D-9D65-EE6D7EF495AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9EE5A-10EF-C04F-A501-CD8F7B202978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2840" windowWidth="27960" windowHeight="18960" xr2:uid="{1440CA57-83F6-A845-B4CA-3C83F36CD9BB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{6DC237D1-36E1-5641-BC25-7F397F77A24A}" name="vspeeds" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/weber/Desktop/vspeeds.csv" comma="1">
+    <textPr sourceFile="/Users/weber/Desktop/vspeeds.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
   <si>
     <t>BEFORE START</t>
   </si>
@@ -234,9 +234,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>Hatches &amp; harnasses</t>
-  </si>
-  <si>
     <t>COMPLETE</t>
   </si>
   <si>
@@ -261,12 +258,6 @@
     <t>SUFFICIENT</t>
   </si>
   <si>
-    <t>BRAKES</t>
-  </si>
-  <si>
-    <t>MASTER</t>
-  </si>
-  <si>
     <t>Pre-flight inspection</t>
   </si>
   <si>
@@ -315,9 +306,6 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>Altimiter</t>
-  </si>
-  <si>
     <t>1013/QNH</t>
   </si>
   <si>
@@ -369,9 +357,6 @@
     <t>IDLE CUT OFF</t>
   </si>
   <si>
-    <t>EFIS &amp; EFIS BACKUP</t>
-  </si>
-  <si>
     <t>OFF AND REMOVE KEY</t>
   </si>
   <si>
@@ -430,6 +415,15 @@
   </si>
   <si>
     <t>SPEEDS</t>
+  </si>
+  <si>
+    <t>Hatches &amp; harnesses</t>
+  </si>
+  <si>
+    <t>Altimeter</t>
+  </si>
+  <si>
+    <t>EFIS &amp; EFIS Backup</t>
   </si>
 </sst>
 </file>
@@ -555,19 +549,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -708,758 +702,6 @@
         </patternFill>
       </fill>
       <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1476,6 +718,26 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1497,6 +759,74 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4"/>
@@ -1504,6 +834,62 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4"/>
@@ -1511,11 +897,115 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1532,6 +1022,26 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1553,10 +1063,141 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1602,6 +1243,39 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -1638,6 +1312,191 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1653,6 +1512,34 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1662,7 +1549,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -1674,10 +1561,15 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
         <right/>
-        <top/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -1714,6 +1606,69 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -1728,6 +1683,45 @@
           <color theme="4"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1747,120 +1741,120 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B687FF71-3DE6-7A4A-8883-34196D3A6A90}" name="Table4" displayName="Table4" ref="A2:B15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B687FF71-3DE6-7A4A-8883-34196D3A6A90}" name="Table4" displayName="Table4" ref="A2:B15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB9E540C-8D52-0344-98EC-3ECCC0A9CB95}" name="Column1" headerRowDxfId="64" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{C7D78C0A-2FD3-9443-B3D4-712D8D7B59A8}" name="Column2" headerRowDxfId="65" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{FB9E540C-8D52-0344-98EC-3ECCC0A9CB95}" name="Column1" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{C7D78C0A-2FD3-9443-B3D4-712D8D7B59A8}" name="Column2" headerRowDxfId="61" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{ED571318-A662-0444-8DF9-9335ABF6BA1D}" name="Table18" displayName="Table18" ref="D45:E49" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{ED571318-A662-0444-8DF9-9335ABF6BA1D}" name="Table18" displayName="Table18" ref="D45:E49" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F2476105-7653-8A4A-BB4D-9734B98CAFD7}" name="Column1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{5C70E72B-2C8B-5443-B280-0C31184053F1}" name="Column2" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F2476105-7653-8A4A-BB4D-9734B98CAFD7}" name="Column1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{5C70E72B-2C8B-5443-B280-0C31184053F1}" name="Column2" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{CB83D555-21A0-2347-8E8A-67D0DF726AEC}" name="Table19" displayName="Table19" ref="D52:E59" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{CB83D555-21A0-2347-8E8A-67D0DF726AEC}" name="Table19" displayName="Table19" ref="D52:E59" headerRowCount="0" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FAED080F-5C51-3744-AFC8-4C43520CDE8C}" name="Column1" headerRowDxfId="50" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{AA1DBD01-BF48-9047-BDE8-75AFE26ACCD1}" name="Column2" headerRowDxfId="51" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{FAED080F-5C51-3744-AFC8-4C43520CDE8C}" name="Column1" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{AA1DBD01-BF48-9047-BDE8-75AFE26ACCD1}" name="Column2" headerRowDxfId="7" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AA9C23E8-DF2B-CA48-9617-6F51FB88ABCC}" name="Table20" displayName="Table20" ref="A62:B69" headerRowCount="0" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AA9C23E8-DF2B-CA48-9617-6F51FB88ABCC}" name="Table20" displayName="Table20" ref="A62:B69" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B279869B-6126-DD47-B9D0-B347A3B5ACE1}" name="Column1" headerRowDxfId="0" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3FA1E4B3-53A0-954D-B5D1-91EACF5259A2}" name="Column2" headerRowDxfId="1" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{B279869B-6126-DD47-B9D0-B347A3B5ACE1}" name="Column1" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3FA1E4B3-53A0-954D-B5D1-91EACF5259A2}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2C3FFF94-473F-EC4F-90DB-028BE695FCD5}" name="Table7" displayName="Table7" ref="A18:B24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2C3FFF94-473F-EC4F-90DB-028BE695FCD5}" name="Table7" displayName="Table7" ref="A18:B24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{59FA7303-8EBF-2B4F-8709-575351C56BDF}" name="Column1" headerRowDxfId="63" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{D6EBC5C3-09E2-274C-AFEC-574B82C53044}" name="Column2" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{59FA7303-8EBF-2B4F-8709-575351C56BDF}" name="Column1" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{D6EBC5C3-09E2-274C-AFEC-574B82C53044}" name="Column2" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{21A87481-F44D-074C-A4BB-B84CD7F0BBA2}" name="Table8" displayName="Table8" ref="A27:B28" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{21A87481-F44D-074C-A4BB-B84CD7F0BBA2}" name="Table8" displayName="Table8" ref="A27:B28" headerRowCount="0" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{29D20034-FF96-3349-BE59-0BDD04CF9F15}" name="Column1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{0AF161EC-7FAB-AC4C-B18F-09AF510852A2}" name="Column2" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{29D20034-FF96-3349-BE59-0BDD04CF9F15}" name="Column1" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{0AF161EC-7FAB-AC4C-B18F-09AF510852A2}" name="Column2" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{39C7865F-47CA-3D41-AE29-C0363E229349}" name="Table11" displayName="Table11" ref="A31:B59" headerRowCount="0" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{39C7865F-47CA-3D41-AE29-C0363E229349}" name="Table11" displayName="Table11" ref="A31:B59" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{746505A2-2E45-D34C-B3B1-EAF7CEB51EF0}" name="Column1" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{D85A58A8-FBDB-824A-BB78-1549392D001F}" name="Column2" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{746505A2-2E45-D34C-B3B1-EAF7CEB51EF0}" name="Column1" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{D85A58A8-FBDB-824A-BB78-1549392D001F}" name="Column2" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CA52DA0-6FDC-2C48-9B6E-9E59A64B1DA1}" name="Table413" displayName="Table413" ref="D2:E6" headerRowCount="0" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4CA52DA0-6FDC-2C48-9B6E-9E59A64B1DA1}" name="Table413" displayName="Table413" ref="D2:E6" headerRowCount="0" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{711FF988-B131-184C-A563-C4A7455D9ED9}" name="Column1" headerRowDxfId="61" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{3121EFA1-B491-5943-9352-854BCAB895B1}" name="Column2" headerRowDxfId="60" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{711FF988-B131-184C-A563-C4A7455D9ED9}" name="Column1" headerRowDxfId="43" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{3121EFA1-B491-5943-9352-854BCAB895B1}" name="Column2" headerRowDxfId="41" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A2641364-7B00-FF45-B7D7-C163B541E6FA}" name="Table13" displayName="Table13" ref="D9:E16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A2641364-7B00-FF45-B7D7-C163B541E6FA}" name="Table13" displayName="Table13" ref="D9:E16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{233672BD-465B-A94A-B79E-D0A57C1D7582}" name="Column1" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{FE8C1779-FC02-1943-8ED9-5BEBBFFDC507}" name="Column2" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{233672BD-465B-A94A-B79E-D0A57C1D7582}" name="Column1" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{FE8C1779-FC02-1943-8ED9-5BEBBFFDC507}" name="Column2" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{271E0835-57F3-DB41-9D80-B418CF104E78}" name="Table15" displayName="Table15" ref="D19:E24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{271E0835-57F3-DB41-9D80-B418CF104E78}" name="Table15" displayName="Table15" ref="D19:E24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CCE16D1A-1707-224A-9770-0C41FC197273}" name="Column1" headerRowDxfId="56" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{35BE18CA-71D3-0843-A2D4-E44296D3415C}" name="Column2" headerRowDxfId="57" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{CCE16D1A-1707-224A-9770-0C41FC197273}" name="Column1" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{35BE18CA-71D3-0843-A2D4-E44296D3415C}" name="Column2" headerRowDxfId="29" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C87ECFBE-457D-904F-B877-FADC4E28E839}" name="Table16" displayName="Table16" ref="D27:E35" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C87ECFBE-457D-904F-B877-FADC4E28E839}" name="Table16" displayName="Table16" ref="D27:E35" headerRowCount="0" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{538ADED3-7A81-DB4E-B5F3-654DBB3AB7C0}" name="Column1" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{77827F5E-7547-C24F-9FDC-CD9D71599726}" name="Column2" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{538ADED3-7A81-DB4E-B5F3-654DBB3AB7C0}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{77827F5E-7547-C24F-9FDC-CD9D71599726}" name="Column2" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4D739757-D692-0E42-B061-F1C8CF3A4345}" name="Table17" displayName="Table17" ref="D38:E42" headerRowCount="0" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4D739757-D692-0E42-B061-F1C8CF3A4345}" name="Table17" displayName="Table17" ref="D38:E42" headerRowCount="0" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{443FCC10-3516-F241-AEE2-0E8CE8387816}" name="Column1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{7A9ABE92-A0A7-EB49-9522-DE12C41CEA9F}" name="Column2" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{443FCC10-3516-F241-AEE2-0E8CE8387816}" name="Column1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{7A9ABE92-A0A7-EB49-9522-DE12C41CEA9F}" name="Column2" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2169,7 +2163,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2178,24 +2172,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="D1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -2209,10 +2203,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2237,7 +2231,7 @@
         <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -2251,7 +2245,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>3</v>
@@ -2273,7 +2267,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E8" s="10"/>
     </row>
@@ -2288,7 +2282,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2299,10 +2293,10 @@
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2316,7 +2310,7 @@
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2324,13 +2318,13 @@
         <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2358,7 +2352,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2379,17 +2373,17 @@
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -2399,7 +2393,7 @@
         <v>46</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E18" s="10"/>
     </row>
@@ -2414,7 +2408,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2439,7 +2433,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>5</v>
@@ -2453,7 +2447,7 @@
         <v>28</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>19</v>
@@ -2467,10 +2461,10 @@
         <v>30</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2481,25 +2475,25 @@
         <v>5</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="11"/>
       <c r="D26" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>37</v>
@@ -2519,10 +2513,10 @@
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2530,14 +2524,14 @@
         <v>18</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="11"/>
       <c r="D30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2575,7 +2569,7 @@
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>45</v>
@@ -2595,7 +2589,7 @@
         <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>3</v>
@@ -2609,7 +2603,7 @@
         <v>30</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>7</v>
@@ -2631,7 +2625,7 @@
         <v>49</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -2643,10 +2637,10 @@
         <v>50</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2674,7 +2668,7 @@
         <v>14</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2699,44 +2693,44 @@
         <v>46</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>109</v>
+      <c r="A43" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D44" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2747,7 +2741,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>10</v>
@@ -2764,7 +2758,7 @@
         <v>14</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2775,7 +2769,7 @@
         <v>19</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
@@ -2808,10 +2802,10 @@
         <v>13</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E51" s="10"/>
     </row>
@@ -2831,7 +2825,7 @@
     </row>
     <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>19</v>
@@ -2840,7 +2834,7 @@
         <v>42</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2868,7 +2862,7 @@
         <v>29</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2882,12 +2876,12 @@
         <v>18</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>60</v>
@@ -2896,18 +2890,18 @@
         <v>29</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>10</v>
@@ -2918,10 +2912,10 @@
         <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>10</v>
@@ -2932,119 +2926,124 @@
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" s="12"/>
+      <c r="A61" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D44:E44"/>
@@ -3052,11 +3051,6 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update checklists, stall speeds and correct spelling errors
</commit_message>
<xml_diff>
--- a/CHECKLIST.xlsx
+++ b/CHECKLIST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weber/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weber/Desktop/Work/RV7POH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9EE5A-10EF-C04F-A501-CD8F7B202978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D3E7A0-5097-7940-873E-E8FDDE51089F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2840" windowWidth="27960" windowHeight="18960" xr2:uid="{1440CA57-83F6-A845-B4CA-3C83F36CD9BB}"/>
+    <workbookView xWindow="440" yWindow="4900" windowWidth="27960" windowHeight="18960" xr2:uid="{1440CA57-83F6-A845-B4CA-3C83F36CD9BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Base!$A$1:$E$69</definedName>
     <definedName name="vspeeds" localSheetId="0">Base!$G$62:$I$68</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>BEFORE START</t>
   </si>
@@ -526,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -552,17 +552,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1771,7 +1774,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AA9C23E8-DF2B-CA48-9617-6F51FB88ABCC}" name="Table20" displayName="Table20" ref="A62:B69" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AA9C23E8-DF2B-CA48-9617-6F51FB88ABCC}" name="Table20" displayName="Table20" ref="A63:B70" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B279869B-6126-DD47-B9D0-B347A3B5ACE1}" name="Column1" headerRowDxfId="3" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{3FA1E4B3-53A0-954D-B5D1-91EACF5259A2}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
@@ -1781,7 +1784,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2C3FFF94-473F-EC4F-90DB-028BE695FCD5}" name="Table7" displayName="Table7" ref="A18:B24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2C3FFF94-473F-EC4F-90DB-028BE695FCD5}" name="Table7" displayName="Table7" ref="A18:B25" headerRowCount="0" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{59FA7303-8EBF-2B4F-8709-575351C56BDF}" name="Column1" headerRowDxfId="57" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{D6EBC5C3-09E2-274C-AFEC-574B82C53044}" name="Column2" dataDxfId="55"/>
@@ -1791,7 +1794,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{21A87481-F44D-074C-A4BB-B84CD7F0BBA2}" name="Table8" displayName="Table8" ref="A27:B28" headerRowCount="0" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{21A87481-F44D-074C-A4BB-B84CD7F0BBA2}" name="Table8" displayName="Table8" ref="A28:B29" headerRowCount="0" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{29D20034-FF96-3349-BE59-0BDD04CF9F15}" name="Column1" dataDxfId="52"/>
     <tableColumn id="2" xr3:uid="{0AF161EC-7FAB-AC4C-B18F-09AF510852A2}" name="Column2" dataDxfId="51"/>
@@ -1801,7 +1804,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{39C7865F-47CA-3D41-AE29-C0363E229349}" name="Table11" displayName="Table11" ref="A31:B59" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{39C7865F-47CA-3D41-AE29-C0363E229349}" name="Table11" displayName="Table11" ref="A32:B60" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{746505A2-2E45-D34C-B3B1-EAF7CEB51EF0}" name="Column1" dataDxfId="48"/>
     <tableColumn id="2" xr3:uid="{D85A58A8-FBDB-824A-BB78-1549392D001F}" name="Column2" dataDxfId="47"/>
@@ -2160,26 +2163,28 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="32.33203125" style="1"/>
+    <col min="1" max="2" width="32.33203125" style="1"/>
+    <col min="3" max="3" width="12" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="32.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2300,10 +2305,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2328,10 +2333,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2356,10 +2361,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2380,10 +2385,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -2468,11 +2473,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>86</v>
@@ -2481,23 +2486,25 @@
         <v>5</v>
       </c>
     </row>
+    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="11"/>
       <c r="D26" s="10" t="s">
         <v>87</v>
       </c>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="12"/>
       <c r="D27" s="1" t="s">
         <v>34</v>
       </c>
@@ -2507,10 +2514,10 @@
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>78</v>
@@ -2520,6 +2527,12 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2528,10 +2541,6 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="11"/>
       <c r="D30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2540,12 +2549,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="12"/>
       <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2555,10 +2562,10 @@
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>58</v>
@@ -2569,10 +2576,10 @@
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>14</v>
@@ -2583,10 +2590,10 @@
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>81</v>
@@ -2597,10 +2604,10 @@
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>122</v>
@@ -2611,18 +2618,18 @@
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>91</v>
@@ -2631,10 +2638,10 @@
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>78</v>
@@ -2645,10 +2652,10 @@
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>48</v>
@@ -2659,10 +2666,10 @@
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>14</v>
@@ -2673,10 +2680,10 @@
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>58</v>
@@ -2687,10 +2694,10 @@
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>93</v>
@@ -2700,19 +2707,19 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>94</v>
@@ -2721,10 +2728,10 @@
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>72</v>
@@ -2735,10 +2742,10 @@
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>96</v>
@@ -2749,10 +2756,10 @@
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>14</v>
@@ -2763,10 +2770,10 @@
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>97</v>
@@ -2777,10 +2784,10 @@
     </row>
     <row r="49" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>18</v>
@@ -2791,18 +2798,18 @@
     </row>
     <row r="50" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>98</v>
@@ -2811,10 +2818,10 @@
     </row>
     <row r="52" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>48</v>
@@ -2825,7 +2832,7 @@
     </row>
     <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>19</v>
@@ -2839,10 +2846,10 @@
     </row>
     <row r="54" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>9</v>
@@ -2853,7 +2860,7 @@
     </row>
     <row r="55" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>3</v>
@@ -2867,10 +2874,10 @@
     </row>
     <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>18</v>
@@ -2881,10 +2888,10 @@
     </row>
     <row r="57" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>29</v>
@@ -2895,10 +2902,10 @@
     </row>
     <row r="58" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>124</v>
@@ -2909,10 +2916,10 @@
     </row>
     <row r="59" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>12</v>
@@ -2922,22 +2929,20 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B62" s="11"/>
       <c r="H62" s="1" t="s">
         <v>114</v>
       </c>
@@ -2947,10 +2952,10 @@
     </row>
     <row r="63" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>115</v>
@@ -2961,10 +2966,10 @@
     </row>
     <row r="64" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>116</v>
@@ -2975,10 +2980,10 @@
     </row>
     <row r="65" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>117</v>
@@ -2989,10 +2994,10 @@
     </row>
     <row r="66" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>118</v>
@@ -3003,10 +3008,10 @@
     </row>
     <row r="67" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>119</v>
@@ -3017,10 +3022,10 @@
     </row>
     <row r="68" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>120</v>
@@ -3031,29 +3036,41 @@
     </row>
     <row r="69" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="E70" s="13">
+        <f ca="1">TODAY()</f>
+        <v>43758</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="12">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Fix spreadsheet print area
</commit_message>
<xml_diff>
--- a/CHECKLIST.xlsx
+++ b/CHECKLIST.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weber/Desktop/Work/RV7POH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D3E7A0-5097-7940-873E-E8FDDE51089F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91BF362-8AB4-A34E-8AE9-253F96BD432E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="4900" windowWidth="27960" windowHeight="18960" xr2:uid="{1440CA57-83F6-A845-B4CA-3C83F36CD9BB}"/>
+    <workbookView xWindow="440" yWindow="2500" windowWidth="27960" windowHeight="21360" xr2:uid="{1440CA57-83F6-A845-B4CA-3C83F36CD9BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Base!$A$1:$E$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Base!$A$1:$E$70</definedName>
     <definedName name="vspeeds" localSheetId="0">Base!$G$62:$I$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="126">
   <si>
     <t>BEFORE START</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>EFIS &amp; EFIS Backup</t>
+  </si>
+  <si>
+    <t>Date of issue</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,8 +487,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -507,15 +516,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -526,18 +546,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -552,19 +572,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2163,10 +2186,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2177,20 +2200,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2271,10 +2294,10 @@
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -2388,7 +2411,7 @@
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -2397,10 +2420,10 @@
       <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
@@ -2495,16 +2518,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="13"/>
       <c r="D27" s="1" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2575,7 @@
       <c r="A31" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="13"/>
       <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2631,10 +2654,10 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -2721,10 +2744,10 @@
       <c r="B44" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="10"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -2782,7 +2805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>18</v>
       </c>
@@ -2796,7 +2819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2804,19 +2827,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
@@ -2830,7 +2853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -2844,7 +2867,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -2858,7 +2881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -2872,7 +2895,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -2886,7 +2909,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
@@ -2900,7 +2923,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -2914,7 +2937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>122</v>
       </c>
@@ -2928,7 +2951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
@@ -2938,103 +2961,61 @@
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
+    <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="H62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="9"/>
+    </row>
+    <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>119</v>
       </c>
@@ -3042,14 +3023,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E70" s="13">
+      <c r="D70" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" s="14">
         <f ca="1">TODAY()</f>
         <v>43758</v>
       </c>

</xml_diff>